<commit_message>
single cycle core ported to basic riscv isa
</commit_message>
<xml_diff>
--- a/scalar_cores/5stage_core/docs/instructions.xlsx
+++ b/scalar_cores/5stage_core/docs/instructions.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NCSU_classes_files\spring20\633\Project\Heterogeneous-multicore\my_5_stage_proc\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NCSU_classes_files\spring20\633\Project\HMP\Heterogeneous-multicore\scalar_cores\5stage_core\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0019F4-C85C-4BC7-B562-9C4A4AC77274}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE3CAD1-4C96-4FF8-8E32-A89EE84B9665}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="369" activeTab="1" xr2:uid="{718E7806-298C-4F07-8385-55875B93F518}"/>
   </bookViews>
   <sheets>
-    <sheet name="ISA" sheetId="1" r:id="rId1"/>
-    <sheet name="mipstest" sheetId="2" r:id="rId2"/>
+    <sheet name="Harris book ISA" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="mipstest" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="177">
   <si>
     <t>RTYPE</t>
   </si>
@@ -481,6 +482,90 @@
   </si>
   <si>
     <t>DATA</t>
+  </si>
+  <si>
+    <t>instn</t>
+  </si>
+  <si>
+    <t>instn type</t>
+  </si>
+  <si>
+    <t>funct7</t>
+  </si>
+  <si>
+    <t>rs2</t>
+  </si>
+  <si>
+    <t>rs1</t>
+  </si>
+  <si>
+    <t>funct3</t>
+  </si>
+  <si>
+    <t>rd</t>
+  </si>
+  <si>
+    <t>opcode</t>
+  </si>
+  <si>
+    <t>R-type</t>
+  </si>
+  <si>
+    <t>imm[11:0]</t>
+  </si>
+  <si>
+    <t>I-type</t>
+  </si>
+  <si>
+    <t>imm[11:5]</t>
+  </si>
+  <si>
+    <t>imm[4:0]</t>
+  </si>
+  <si>
+    <t>S-type</t>
+  </si>
+  <si>
+    <t>B-type</t>
+  </si>
+  <si>
+    <t>imm[31:12]</t>
+  </si>
+  <si>
+    <t>U-type</t>
+  </si>
+  <si>
+    <t>J-type</t>
+  </si>
+  <si>
+    <t>[6:0]</t>
+  </si>
+  <si>
+    <t>[11:7]</t>
+  </si>
+  <si>
+    <t>[14:12]</t>
+  </si>
+  <si>
+    <t>[19:15]</t>
+  </si>
+  <si>
+    <t>[24:20]</t>
+  </si>
+  <si>
+    <t>[31:25]</t>
+  </si>
+  <si>
+    <t>imm[4:1] imm[11]</t>
+  </si>
+  <si>
+    <t>imm[12 ]imm[10:5]</t>
+  </si>
+  <si>
+    <t>imm[20]  imm[10:1]  imm[11]</t>
+  </si>
+  <si>
+    <t>imm[19:12]</t>
   </si>
 </sst>
 </file>
@@ -616,7 +701,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -663,10 +748,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -676,12 +770,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1000,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{268BA47F-AF47-4F29-ABE4-FB53CAF89061}">
   <dimension ref="B2:Q44"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,18 +1103,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
@@ -1274,18 +1362,18 @@
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
@@ -1352,20 +1440,20 @@
       <c r="I13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J13" s="26" t="s">
+      <c r="J13" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26" t="s">
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
-      <c r="P13" s="26" t="s">
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="Q13" s="26"/>
+      <c r="Q13" s="28"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
@@ -1374,14 +1462,14 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="28"/>
-      <c r="Q14" s="28"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="31"/>
+      <c r="Q14" s="31"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
@@ -1433,25 +1521,25 @@
       <c r="F16" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="26" t="s">
+      <c r="G16" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26" t="s">
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26" t="s">
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
-      <c r="P16" s="26" t="s">
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="Q16" s="26"/>
+      <c r="Q16" s="28"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" s="14">
@@ -1469,25 +1557,25 @@
       <c r="F17" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="G17" s="26" t="s">
+      <c r="G17" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26" t="s">
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26" t="s">
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26" t="s">
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="Q17" s="26"/>
+      <c r="Q17" s="28"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="14">
@@ -1505,25 +1593,25 @@
       <c r="F18" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="G18" s="26" t="s">
+      <c r="G18" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26" t="s">
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="26" t="s">
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="N18" s="26"/>
-      <c r="O18" s="26"/>
-      <c r="P18" s="26" t="s">
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="Q18" s="26"/>
+      <c r="Q18" s="28"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="14">
@@ -1541,36 +1629,36 @@
       <c r="F19" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="26" t="s">
+      <c r="G19" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26" t="s">
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26" t="s">
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
-      <c r="P19" s="26" t="s">
+      <c r="N19" s="28"/>
+      <c r="O19" s="28"/>
+      <c r="P19" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="Q19" s="26"/>
+      <c r="Q19" s="28"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="28"/>
-      <c r="O20" s="28"/>
-      <c r="P20" s="28"/>
-      <c r="Q20" s="28"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="31"/>
+      <c r="P20" s="31"/>
+      <c r="Q20" s="31"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
@@ -1612,32 +1700,32 @@
       <c r="D22" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="E22" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26" t="s">
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="K22" s="26"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="26" t="s">
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="N22" s="26"/>
-      <c r="O22" s="32"/>
-      <c r="P22" s="31" t="s">
+      <c r="N22" s="28"/>
+      <c r="O22" s="30"/>
+      <c r="P22" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="Q22" s="31"/>
+      <c r="Q22" s="29"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
-      <c r="P23" s="31"/>
-      <c r="Q23" s="31"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="29"/>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C24" s="23" t="s">
@@ -1784,6 +1872,32 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="C11:L11"/>
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="M17:O17"/>
     <mergeCell ref="E21:I21"/>
     <mergeCell ref="E22:I22"/>
     <mergeCell ref="P22:Q23"/>
@@ -1800,32 +1914,6 @@
     <mergeCell ref="P20:Q20"/>
     <mergeCell ref="P21:Q21"/>
     <mergeCell ref="J22:L22"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="M18:O18"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="C2:L2"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="C11:L11"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="J15:L15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1834,10 +1922,197 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8B24B8-6F90-4495-86A9-827C67D60825}">
+  <dimension ref="B2:H15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="26"/>
+    <col min="2" max="2" width="22.140625" style="26" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="26" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="26" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="26" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" style="26" customWidth="1"/>
+    <col min="7" max="7" width="12" style="26" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="26"/>
+    <col min="9" max="9" width="24.5703125" style="26" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="26"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="H3" s="26" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="C4" s="31"/>
+      <c r="D4" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="E8" s="31"/>
+      <c r="F8" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="H8" s="26" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC80CC1-2568-45BC-8C8F-5C49C714F2FC}">
   <dimension ref="A4:AE22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>

</xml_diff>